<commit_message>
Mudanças no banco de dados e alterações gerais no site
</commit_message>
<xml_diff>
--- a/ASSISTENCIA/Tabela Riscos.xlsx
+++ b/ASSISTENCIA/Tabela Riscos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corin\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corin\OneDrive\Área de Trabalho\Nova pasta (3)\projeto-pi-2sprint\ASSISTENCIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60EEF204-5959-4FA6-A6BB-0FB6358B7CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA9855D-4891-4634-904C-3AEBA95438D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2A551E82-236B-4B87-98C8-830F711640C6}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>Falta de Comprometimento</t>
   </si>
   <si>
-    <t>Dividino as tarefas com os membros restantes do grupo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cobrando e conversando com a pessoa </t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>Utilizando ferramentas de gestão e as atualizando conforme o progresso das reuniões</t>
+  </si>
+  <si>
+    <t>Dividindo as tarefas com os membros restantes do grupo</t>
   </si>
 </sst>
 </file>
@@ -306,27 +306,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,9 +321,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -354,15 +333,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -370,6 +340,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -692,7 +692,7 @@
   <dimension ref="B2:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O6"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,156 +714,156 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="2:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="17">
-        <v>3</v>
-      </c>
-      <c r="D3" s="19">
+      <c r="C3" s="10">
+        <v>3</v>
+      </c>
+      <c r="D3" s="12">
         <v>6</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="12">
         <v>9</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="24"/>
+      <c r="R3" s="14"/>
     </row>
     <row r="4" spans="2:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="11">
         <v>2</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="10">
         <v>4</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="12">
         <v>6</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="4"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="18"/>
       <c r="M4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="24"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="14"/>
     </row>
     <row r="5" spans="2:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="11">
         <v>2</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="10">
         <v>3</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="4"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="18"/>
       <c r="M5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="25" t="s">
+      <c r="O5" s="18"/>
+      <c r="P5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="24"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="14"/>
     </row>
     <row r="6" spans="2:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="14" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="11" t="s">
+      <c r="K6" s="25"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="26" t="s">
+      <c r="O6" s="26"/>
+      <c r="P6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="24"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="14"/>
     </row>
     <row r="7" spans="2:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -883,19 +883,19 @@
       <c r="O7" s="3">
         <v>6</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="P7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="R7" s="23"/>
+      <c r="Q7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="13"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K8" s="3">
         <v>2</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="L8" s="13" t="s">
         <v>22</v>
       </c>
       <c r="M8" s="3">
@@ -907,20 +907,20 @@
       <c r="O8" s="3">
         <v>3</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="P8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="R8" s="23"/>
+      <c r="Q8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="13"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K9" s="3">
         <v>3</v>
       </c>
-      <c r="L9" s="23" t="s">
-        <v>25</v>
+      <c r="L9" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="M9" s="3">
         <v>2</v>
@@ -934,17 +934,17 @@
       <c r="P9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="23"/>
+      <c r="Q9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="R9" s="13"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K10" s="3">
         <v>4</v>
       </c>
       <c r="L10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M10" s="3">
         <v>2</v>
@@ -958,17 +958,17 @@
       <c r="P10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" s="23"/>
+      <c r="Q10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="R10" s="13"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K11" s="3">
         <v>5</v>
       </c>
       <c r="L11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M11" s="3">
         <v>1</v>
@@ -982,17 +982,17 @@
       <c r="P11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q11" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="R11" s="23"/>
+      <c r="Q11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="13"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K12" s="3">
         <v>6</v>
       </c>
       <c r="L12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M12" s="3">
         <v>1</v>
@@ -1006,17 +1006,17 @@
       <c r="P12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q12" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="R12" s="23"/>
+      <c r="Q12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" s="13"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K13" s="3">
         <v>7</v>
       </c>
       <c r="L13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M13" s="3">
         <v>2</v>
@@ -1030,10 +1030,10 @@
       <c r="P13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q13" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="R13" s="23"/>
+      <c r="Q13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="R13" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>